<commit_message>
Update Vite configuration and enhance file download functionality
- Added support for including Excel and CSV files in the Vite build process.
- Updated EngineersList and ModelList components to use imported sample files for download links, improving code clarity and maintainability.
- Adjusted download button functionality to reference the imported file paths directly.
</commit_message>
<xml_diff>
--- a/src/assets/sample.xlsx
+++ b/src/assets/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrsou\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9449AFF7-7DCE-4240-8313-F308DD61F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE33A021-27CA-4212-8F45-261C12A822B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>longitude</t>
   </si>
   <si>
-    <t>brand_id</t>
-  </si>
-  <si>
     <t>expertise_id</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
   </si>
   <si>
     <t>India</t>
-  </si>
-  <si>
-    <t>7,10</t>
   </si>
   <si>
     <t>2,3</t>
@@ -150,12 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,7 +459,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,37 +499,35 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D2">
         <v>9632587410</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
       <c r="I2">
         <v>22.7286</v>
@@ -543,10 +536,7 @@
         <v>75.895799999999994</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>